<commit_message>
Got a first finished build here. Outputs to an excel file with the summary of the files
</commit_message>
<xml_diff>
--- a/output/Summary of Files.xlsx
+++ b/output/Summary of Files.xlsx
@@ -14,7 +14,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
+  <si>
+    <t>Workbook</t>
+  </si>
+  <si>
+    <t># sheets</t>
+  </si>
+  <si>
+    <t>Sheetname</t>
+  </si>
+  <si>
+    <t>Rows</t>
+  </si>
+  <si>
+    <t>Columns</t>
+  </si>
+  <si>
+    <t>Workbook Size</t>
+  </si>
+  <si>
+    <t>Useful(1-5)</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
   <si>
     <t>Cars.xls</t>
   </si>
@@ -393,7 +417,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -403,182 +427,208 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1">
-        <v>1729</v>
-      </c>
-      <c r="E1">
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
         <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1">
-        <v>0</v>
-      </c>
-      <c r="H1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B2">
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D2">
-        <v>15</v>
+        <v>1729</v>
       </c>
       <c r="E2">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F3" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D4">
-        <v>155</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D5">
-        <v>28</v>
+        <v>155</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6">
+        <v>28</v>
+      </c>
+      <c r="E6">
         <v>1</v>
       </c>
-      <c r="C6" t="s">
+      <c r="F6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
         <v>11</v>
-      </c>
-      <c r="D6">
-        <v>101</v>
-      </c>
-      <c r="E6">
-        <v>3</v>
-      </c>
-      <c r="F6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D7">
+        <v>101</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8">
         <v>1501</v>
       </c>
-      <c r="E7">
+      <c r="E8">
         <v>6</v>
       </c>
-      <c r="F7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7" t="s">
-        <v>3</v>
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>